<commit_message>
feat(belanja-item): add command regenerate belanja items
</commit_message>
<xml_diff>
--- a/resources/excel/testing_regen.xlsx
+++ b/resources/excel/testing_regen.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48916E3A-D971-453B-A2BA-E0C6885CA359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C708342-62C2-474F-AC7B-6FD682F2294F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Lokasi : KOTA JAKARTA SELATAN</t>
   </si>
@@ -60,13 +60,70 @@
   </si>
   <si>
     <t>Penyusunan Bahan Kerja Sama HAM</t>
+  </si>
+  <si>
+    <t>Belanja Bahan</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>(KPPN.139-Jakarta V )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - </t>
+  </si>
+  <si>
+    <t>ATK</t>
+  </si>
+  <si>
+    <t>1.0 THN</t>
+  </si>
+  <si>
+    <t>Penggandaan dan Penjilidan Laporan</t>
+  </si>
+  <si>
+    <t>6.0 BK</t>
+  </si>
+  <si>
+    <t>KUDAPAN RAPAT [15 ORG x 10 KEG]</t>
+  </si>
+  <si>
+    <t>150.0 OK</t>
+  </si>
+  <si>
+    <t>MAKAN RAPAT [15 ORG x 10 KEG]</t>
+  </si>
+  <si>
+    <t>SEMINAR KIT</t>
+  </si>
+  <si>
+    <t>1.0 KEG</t>
+  </si>
+  <si>
+    <t>522151</t>
+  </si>
+  <si>
+    <t>Belanja Jasa Profesi</t>
+  </si>
+  <si>
+    <t>Honor Narasumber [1 ORG x 2 JAM x 5 KEG]</t>
+  </si>
+  <si>
+    <t>10.0 OJ</t>
+  </si>
+  <si>
+    <t>Honor Narasumber Paket Meeting [4 ORG x 4 JAM x 1 KEG]</t>
+  </si>
+  <si>
+    <t>16.0 OJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +170,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="SansSerif"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="16">
     <fill>
@@ -197,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -227,19 +297,47 @@
     <xf numFmtId="3" fontId="6" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -559,10 +657,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:F5"/>
+      <selection activeCell="H17" sqref="H17:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -582,16 +680,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.05" customHeight="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -603,16 +701,16 @@
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="13.95" customHeight="1">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
@@ -629,11 +727,11 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
       <c r="G3" s="3"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -643,16 +741,16 @@
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="15.6">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
       <c r="G4" s="5" t="s">
         <v>10</v>
       </c>
@@ -666,16 +764,16 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="13.05" customHeight="1">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
       <c r="G5" s="7" t="s">
         <v>3</v>
       </c>
@@ -691,16 +789,16 @@
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" ht="13.05" customHeight="1">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -711,8 +809,256 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="15">
+        <v>521211</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="12">
+        <v>15521000</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="17"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="16">
+        <v>3500000</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="12">
+        <v>3500000</v>
+      </c>
+      <c r="K9" s="11"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="16">
+        <v>252667</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="12">
+        <v>1516000</v>
+      </c>
+      <c r="K10" s="11"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="16">
+        <v>16800</v>
+      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="12">
+        <v>2520000</v>
+      </c>
+      <c r="K11" s="11"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="16">
+        <v>39900</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="12">
+        <v>5985000</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="16">
+        <v>2000000</v>
+      </c>
+      <c r="I13" s="16"/>
+      <c r="J13" s="12">
+        <v>2000000</v>
+      </c>
+      <c r="K13" s="11"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="12">
+        <v>18200000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="16">
+        <v>700000</v>
+      </c>
+      <c r="I16" s="16"/>
+      <c r="J16" s="12">
+        <v>7000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="16">
+        <v>700000</v>
+      </c>
+      <c r="I17" s="16"/>
+      <c r="J17" s="12">
+        <v>11200000</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="37">
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="H16:I16"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="A4:C4"/>
@@ -724,6 +1070,25 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="L13:M13"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>